<commit_message>
pridana tabulka subjective ratings
</commit_message>
<xml_diff>
--- a/subjective_ratings.xlsx
+++ b/subjective_ratings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>TP1</t>
   </si>
@@ -50,9 +50,18 @@
     <t>Nebolo jednoduché zistiť ako postupovať</t>
   </si>
   <si>
+    <t>veľmi jednoduché</t>
+  </si>
+  <si>
     <t>Nebolo jasné čo je treba urobiť</t>
   </si>
   <si>
+    <t>veľmi jasné</t>
+  </si>
+  <si>
+    <t>veľmi nejasné</t>
+  </si>
+  <si>
     <t>Na 3 stranke nebolo jasné ako postupovať ďalej</t>
   </si>
   <si>
@@ -65,7 +74,19 @@
     <t>Chcel/a by som využívať toto rozhranie aj v budúcnosti</t>
   </si>
   <si>
+    <t>veľmi</t>
+  </si>
+  <si>
+    <t>vôbec</t>
+  </si>
+  <si>
     <t>Urobil/a by som veľké zmeny v tomto rozhraní</t>
+  </si>
+  <si>
+    <t>žiadne zmeny</t>
+  </si>
+  <si>
+    <t>veľké zmeny</t>
   </si>
 </sst>
 </file>
@@ -80,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -175,14 +197,14 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:J10"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5612244897959"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
@@ -262,7 +284,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -281,16 +303,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -303,16 +325,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -325,16 +347,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -347,16 +369,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -369,16 +391,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -391,16 +413,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>

</xml_diff>